<commit_message>
diferenciacion entre certificacion anterior e inspeccion anterior
</commit_message>
<xml_diff>
--- a/app/templates/template_rules_1.xlsx
+++ b/app/templates/template_rules_1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1359" uniqueCount="629">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1359" uniqueCount="630">
   <si>
     <t xml:space="preserve">Certificado conformidad MINVU.</t>
   </si>
@@ -239,6 +239,9 @@
   </si>
   <si>
     <t xml:space="preserve">Especificar.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.15.1</t>
   </si>
   <si>
     <t xml:space="preserve">Sala de máquinas o de poleas no reservado sólo a personal autorizado.</t>
@@ -2019,8 +2022,8 @@
   </sheetPr>
   <dimension ref="A1:E325"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A262" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E262" activeCellId="51" sqref="E1:E11 E19 E21 E36 E73 E77 E79 E86 E90 E94 E96:E97 E100:E102 E104 E106 E108:E109 E112:E113 E120:E121 E124 E127 E134:E136 E138:E140 E142 E147:E149 E151:E153 E170:E175 E177:E178 E183 E185:E187 E189 E193:E199 E202 E204 E206:E210 E212:E217 E219 E223 E231 E234:E236 E240:E242 E245 E247:E248 E258 E263:E264 E266 E270 E283 E286 E300 E302 E312 E323:E325 E262"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2556,7 +2559,7 @@
         <v>72</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>41</v>
@@ -2570,10 +2573,10 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>30</v>
@@ -2584,10 +2587,10 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>30</v>
@@ -2598,10 +2601,10 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>30</v>
@@ -2612,10 +2615,10 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>27</v>
@@ -2626,10 +2629,10 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>27</v>
@@ -2640,10 +2643,10 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>27</v>
@@ -2654,10 +2657,10 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>27</v>
@@ -2668,10 +2671,10 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>27</v>
@@ -2682,10 +2685,10 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>27</v>
@@ -2696,10 +2699,10 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>30</v>
@@ -2710,10 +2713,10 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>30</v>
@@ -2724,10 +2727,10 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>27</v>
@@ -2738,10 +2741,10 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>30</v>
@@ -2752,10 +2755,10 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>27</v>
@@ -2766,10 +2769,10 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>30</v>
@@ -2780,10 +2783,10 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>30</v>
@@ -2794,10 +2797,10 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>30</v>
@@ -2808,10 +2811,10 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>30</v>
@@ -2822,10 +2825,10 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>27</v>
@@ -2836,10 +2839,10 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>27</v>
@@ -2850,10 +2853,10 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>41</v>
@@ -2864,10 +2867,10 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>30</v>
@@ -2878,10 +2881,10 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>27</v>
@@ -2892,10 +2895,10 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>30</v>
@@ -2906,10 +2909,10 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>30</v>
@@ -2920,10 +2923,10 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>30</v>
@@ -2934,10 +2937,10 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>41</v>
@@ -2948,10 +2951,10 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>41</v>
@@ -2962,10 +2965,10 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>41</v>
@@ -2976,10 +2979,10 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>41</v>
@@ -2990,10 +2993,10 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>41</v>
@@ -3004,10 +3007,10 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>41</v>
@@ -3018,10 +3021,10 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>30</v>
@@ -3032,10 +3035,10 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>30</v>
@@ -3046,10 +3049,10 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>41</v>
@@ -3060,10 +3063,10 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>27</v>
@@ -3074,10 +3077,10 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>41</v>
@@ -3091,10 +3094,10 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>30</v>
@@ -3105,10 +3108,10 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>30</v>
@@ -3119,10 +3122,10 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>30</v>
@@ -3133,10 +3136,10 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>30</v>
@@ -3150,10 +3153,10 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>30</v>
@@ -3164,10 +3167,10 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>41</v>
@@ -3181,10 +3184,10 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>30</v>
@@ -3195,10 +3198,10 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>30</v>
@@ -3209,10 +3212,10 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>41</v>
@@ -3223,10 +3226,10 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>41</v>
@@ -3237,10 +3240,10 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>41</v>
@@ -3251,10 +3254,10 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>41</v>
@@ -3265,10 +3268,10 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>41</v>
@@ -3279,10 +3282,10 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>41</v>
@@ -3293,10 +3296,10 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>30</v>
@@ -3307,10 +3310,10 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>173</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>30</v>
@@ -3321,10 +3324,10 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>30</v>
@@ -3335,10 +3338,10 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>30</v>
@@ -3349,13 +3352,13 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>3</v>
@@ -3363,10 +3366,10 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>27</v>
@@ -3377,10 +3380,10 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>30</v>
@@ -3391,10 +3394,10 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>27</v>
@@ -3405,10 +3408,10 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>30</v>
@@ -3422,10 +3425,10 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>30</v>
@@ -3436,10 +3439,10 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>41</v>
@@ -3450,10 +3453,10 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>41</v>
@@ -3464,10 +3467,10 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>27</v>
@@ -3478,10 +3481,10 @@
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>27</v>
@@ -3495,10 +3498,10 @@
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>30</v>
@@ -3512,10 +3515,10 @@
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>41</v>
@@ -3526,10 +3529,10 @@
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>41</v>
@@ -3540,10 +3543,10 @@
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>41</v>
@@ -3554,10 +3557,10 @@
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>30</v>
@@ -3571,10 +3574,10 @@
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>41</v>
@@ -3585,10 +3588,10 @@
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>41</v>
@@ -3599,10 +3602,10 @@
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>41</v>
@@ -3613,10 +3616,10 @@
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>30</v>
@@ -3627,10 +3630,10 @@
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>30</v>
@@ -3641,10 +3644,10 @@
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>41</v>
@@ -3655,10 +3658,10 @@
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>41</v>
@@ -3669,10 +3672,10 @@
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>41</v>
@@ -3683,10 +3686,10 @@
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>30</v>
@@ -3697,10 +3700,10 @@
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>41</v>
@@ -3711,10 +3714,10 @@
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>41</v>
@@ -3725,10 +3728,10 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>30</v>
@@ -3739,13 +3742,13 @@
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>3</v>
@@ -3753,10 +3756,10 @@
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>41</v>
@@ -3767,10 +3770,10 @@
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>41</v>
@@ -3784,10 +3787,10 @@
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>27</v>
@@ -3798,10 +3801,10 @@
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>27</v>
@@ -3812,10 +3815,10 @@
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>27</v>
@@ -3829,10 +3832,10 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>27</v>
@@ -3843,13 +3846,13 @@
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>3</v>
@@ -3857,13 +3860,13 @@
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>3</v>
@@ -3874,13 +3877,13 @@
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>3</v>
@@ -3888,10 +3891,10 @@
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>30</v>
@@ -3902,10 +3905,10 @@
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>30</v>
@@ -3916,10 +3919,10 @@
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>30</v>
@@ -3930,10 +3933,10 @@
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>30</v>
@@ -3944,10 +3947,10 @@
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>30</v>
@@ -3958,10 +3961,10 @@
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B134" s="1" t="s">
         <v>263</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>262</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>30</v>
@@ -3972,10 +3975,10 @@
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>27</v>
@@ -3989,10 +3992,10 @@
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>30</v>
@@ -4003,10 +4006,10 @@
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>30</v>
@@ -4017,10 +4020,10 @@
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>41</v>
@@ -4034,10 +4037,10 @@
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>41</v>
@@ -4051,10 +4054,10 @@
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>41</v>
@@ -4068,10 +4071,10 @@
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>41</v>
@@ -4082,13 +4085,13 @@
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D142" s="1" t="s">
         <v>3</v>
@@ -4099,10 +4102,10 @@
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C143" s="1" t="s">
         <v>30</v>
@@ -4113,10 +4116,10 @@
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>30</v>
@@ -4127,10 +4130,10 @@
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>27</v>
@@ -4141,10 +4144,10 @@
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>30</v>
@@ -4155,10 +4158,10 @@
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>30</v>
@@ -4169,10 +4172,10 @@
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>30</v>
@@ -4183,10 +4186,10 @@
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>41</v>
@@ -4197,10 +4200,10 @@
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B150" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="B150" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>41</v>
@@ -4211,10 +4214,10 @@
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>41</v>
@@ -4228,10 +4231,10 @@
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>41</v>
@@ -4242,10 +4245,10 @@
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>41</v>
@@ -4256,10 +4259,10 @@
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>41</v>
@@ -4270,10 +4273,10 @@
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>41</v>
@@ -4284,10 +4287,10 @@
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>41</v>
@@ -4298,10 +4301,10 @@
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>41</v>
@@ -4312,10 +4315,10 @@
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>41</v>
@@ -4326,10 +4329,10 @@
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>41</v>
@@ -4340,10 +4343,10 @@
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C160" s="1" t="s">
         <v>27</v>
@@ -4354,10 +4357,10 @@
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C161" s="1" t="s">
         <v>30</v>
@@ -4368,10 +4371,10 @@
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B162" s="1" t="s">
         <v>318</v>
-      </c>
-      <c r="B162" s="1" t="s">
-        <v>317</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>30</v>
@@ -4382,10 +4385,10 @@
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>41</v>
@@ -4396,10 +4399,10 @@
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>30</v>
@@ -4410,10 +4413,10 @@
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>30</v>
@@ -4424,10 +4427,10 @@
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>30</v>
@@ -4438,10 +4441,10 @@
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>30</v>
@@ -4452,10 +4455,10 @@
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C168" s="1" t="s">
         <v>30</v>
@@ -4466,10 +4469,10 @@
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C169" s="1" t="s">
         <v>30</v>
@@ -4480,10 +4483,10 @@
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C170" s="1" t="s">
         <v>30</v>
@@ -4494,10 +4497,10 @@
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C171" s="1" t="s">
         <v>30</v>
@@ -4511,10 +4514,10 @@
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C172" s="1" t="s">
         <v>27</v>
@@ -4528,10 +4531,10 @@
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C173" s="1" t="s">
         <v>27</v>
@@ -4545,10 +4548,10 @@
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>27</v>
@@ -4559,10 +4562,10 @@
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>27</v>
@@ -4573,10 +4576,10 @@
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="1" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>30</v>
@@ -4587,10 +4590,10 @@
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="1" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>30</v>
@@ -4601,10 +4604,10 @@
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>30</v>
@@ -4618,10 +4621,10 @@
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>30</v>
@@ -4632,10 +4635,10 @@
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C180" s="1" t="s">
         <v>41</v>
@@ -4646,10 +4649,10 @@
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="1" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>30</v>
@@ -4660,10 +4663,10 @@
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>27</v>
@@ -4674,10 +4677,10 @@
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C183" s="1" t="s">
         <v>30</v>
@@ -4688,10 +4691,10 @@
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C184" s="1" t="s">
         <v>30</v>
@@ -4702,10 +4705,10 @@
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="1" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C185" s="1" t="s">
         <v>30</v>
@@ -4719,10 +4722,10 @@
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="1" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C186" s="1" t="s">
         <v>27</v>
@@ -4736,10 +4739,10 @@
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C187" s="1" t="s">
         <v>30</v>
@@ -4753,10 +4756,10 @@
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C188" s="1" t="s">
         <v>27</v>
@@ -4767,10 +4770,10 @@
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C189" s="1" t="s">
         <v>41</v>
@@ -4784,10 +4787,10 @@
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>41</v>
@@ -4798,10 +4801,10 @@
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C191" s="1" t="s">
         <v>30</v>
@@ -4812,10 +4815,10 @@
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="1" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C192" s="1" t="s">
         <v>30</v>
@@ -4826,10 +4829,10 @@
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C193" s="1" t="s">
         <v>41</v>
@@ -4840,10 +4843,10 @@
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="1" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>41</v>
@@ -4854,10 +4857,10 @@
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="1" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>41</v>
@@ -4868,10 +4871,10 @@
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="1" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C196" s="1" t="s">
         <v>41</v>
@@ -4882,10 +4885,10 @@
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="1" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>41</v>
@@ -4896,10 +4899,10 @@
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="1" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C198" s="1" t="s">
         <v>30</v>
@@ -4910,10 +4913,10 @@
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>41</v>
@@ -4927,10 +4930,10 @@
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="1" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>41</v>
@@ -4941,10 +4944,10 @@
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="1" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>30</v>
@@ -4955,10 +4958,10 @@
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="1" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>27</v>
@@ -4969,10 +4972,10 @@
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="1" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>30</v>
@@ -4983,10 +4986,10 @@
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="1" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C204" s="1" t="s">
         <v>30</v>
@@ -4997,10 +5000,10 @@
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="1" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C205" s="1" t="s">
         <v>41</v>
@@ -5011,10 +5014,10 @@
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C206" s="1" t="s">
         <v>30</v>
@@ -5025,10 +5028,10 @@
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="1" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C207" s="1" t="s">
         <v>27</v>
@@ -5042,10 +5045,10 @@
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="1" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C208" s="1" t="s">
         <v>30</v>
@@ -5059,10 +5062,10 @@
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="1" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C209" s="1" t="s">
         <v>30</v>
@@ -5076,10 +5079,10 @@
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>41</v>
@@ -5093,13 +5096,13 @@
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="1" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D211" s="1" t="s">
         <v>3</v>
@@ -5107,10 +5110,10 @@
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="1" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>41</v>
@@ -5121,13 +5124,13 @@
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="1" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E213" s="1" t="s">
         <v>4</v>
@@ -5135,10 +5138,10 @@
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="1" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C214" s="1" t="s">
         <v>41</v>
@@ -5152,10 +5155,10 @@
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="1" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>41</v>
@@ -5169,10 +5172,10 @@
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="1" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C216" s="1" t="s">
         <v>41</v>
@@ -5183,10 +5186,10 @@
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="1" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C217" s="1" t="s">
         <v>41</v>
@@ -5197,10 +5200,10 @@
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="1" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>41</v>
@@ -5211,10 +5214,10 @@
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C219" s="1" t="s">
         <v>41</v>
@@ -5228,10 +5231,10 @@
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="1" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C220" s="1" t="s">
         <v>30</v>
@@ -5242,10 +5245,10 @@
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="1" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C221" s="1" t="s">
         <v>27</v>
@@ -5256,10 +5259,10 @@
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="1" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C222" s="1" t="s">
         <v>30</v>
@@ -5270,10 +5273,10 @@
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>30</v>
@@ -5287,10 +5290,10 @@
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="1" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>27</v>
@@ -5301,10 +5304,10 @@
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="1" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C225" s="1" t="s">
         <v>30</v>
@@ -5315,10 +5318,10 @@
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="1" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C226" s="1" t="s">
         <v>30</v>
@@ -5329,10 +5332,10 @@
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="1" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C227" s="1" t="s">
         <v>41</v>
@@ -5343,10 +5346,10 @@
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="1" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C228" s="1" t="s">
         <v>41</v>
@@ -5357,10 +5360,10 @@
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="B229" s="1" t="s">
         <v>449</v>
-      </c>
-      <c r="B229" s="1" t="s">
-        <v>448</v>
       </c>
       <c r="C229" s="1" t="s">
         <v>41</v>
@@ -5371,10 +5374,10 @@
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="1" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C230" s="1" t="s">
         <v>41</v>
@@ -5385,10 +5388,10 @@
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="1" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>41</v>
@@ -5399,10 +5402,10 @@
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="1" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>30</v>
@@ -5413,10 +5416,10 @@
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="1" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>41</v>
@@ -5427,10 +5430,10 @@
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="1" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>41</v>
@@ -5441,10 +5444,10 @@
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>41</v>
@@ -5455,10 +5458,10 @@
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C236" s="1" t="s">
         <v>41</v>
@@ -5472,10 +5475,10 @@
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="1" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C237" s="1" t="s">
         <v>27</v>
@@ -5486,10 +5489,10 @@
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="1" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C238" s="1" t="s">
         <v>27</v>
@@ -5500,10 +5503,10 @@
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="1" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C239" s="1" t="s">
         <v>27</v>
@@ -5514,13 +5517,13 @@
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="D240" s="1" t="s">
         <v>3</v>
@@ -5531,10 +5534,10 @@
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="1" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C241" s="1" t="s">
         <v>30</v>
@@ -5548,10 +5551,10 @@
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="1" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C242" s="1" t="s">
         <v>41</v>
@@ -5562,10 +5565,10 @@
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="1" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C243" s="1" t="s">
         <v>30</v>
@@ -5576,10 +5579,10 @@
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C244" s="1" t="s">
         <v>30</v>
@@ -5590,10 +5593,10 @@
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="C245" s="1" t="s">
         <v>30</v>
@@ -5604,10 +5607,10 @@
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="1" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C246" s="1" t="s">
         <v>30</v>
@@ -5618,13 +5621,13 @@
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="1" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E247" s="1" t="s">
         <v>4</v>
@@ -5632,13 +5635,13 @@
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="1" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D248" s="1" t="s">
         <v>3</v>
@@ -5649,13 +5652,13 @@
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="1" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D249" s="1" t="s">
         <v>3</v>
@@ -5663,10 +5666,10 @@
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="1" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C250" s="1" t="s">
         <v>41</v>
@@ -5677,10 +5680,10 @@
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="1" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="C251" s="1" t="s">
         <v>41</v>
@@ -5691,10 +5694,10 @@
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="1" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="C252" s="1" t="s">
         <v>41</v>
@@ -5705,10 +5708,10 @@
     </row>
     <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="1" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="C253" s="1" t="s">
         <v>27</v>
@@ -5719,10 +5722,10 @@
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="1" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="C254" s="1" t="s">
         <v>30</v>
@@ -5733,10 +5736,10 @@
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="1" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="C255" s="1" t="s">
         <v>30</v>
@@ -5747,10 +5750,10 @@
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="C256" s="1" t="s">
         <v>41</v>
@@ -5761,10 +5764,10 @@
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="1" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="C257" s="1" t="s">
         <v>41</v>
@@ -5775,10 +5778,10 @@
     </row>
     <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="1" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C258" s="1" t="s">
         <v>41</v>
@@ -5789,10 +5792,10 @@
     </row>
     <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="1" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C259" s="1" t="s">
         <v>41</v>
@@ -5803,10 +5806,10 @@
     </row>
     <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="1" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="C260" s="1" t="s">
         <v>41</v>
@@ -5817,10 +5820,10 @@
     </row>
     <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="1" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="C261" s="1" t="s">
         <v>30</v>
@@ -5831,10 +5834,10 @@
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="1" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="C262" s="1" t="s">
         <v>30</v>
@@ -5845,10 +5848,10 @@
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="1" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="C263" s="1" t="s">
         <v>41</v>
@@ -5862,13 +5865,13 @@
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="1" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D264" s="1" t="s">
         <v>3</v>
@@ -5879,10 +5882,10 @@
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="1" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="C265" s="1" t="s">
         <v>30</v>
@@ -5893,10 +5896,10 @@
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="C266" s="1" t="s">
         <v>41</v>
@@ -5910,10 +5913,10 @@
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="1" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="C267" s="1" t="s">
         <v>27</v>
@@ -5924,10 +5927,10 @@
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="1" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="C268" s="1" t="s">
         <v>30</v>
@@ -5938,10 +5941,10 @@
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="1" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="C269" s="1" t="s">
         <v>30</v>
@@ -5952,10 +5955,10 @@
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="1" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="C270" s="1" t="s">
         <v>30</v>
@@ -5966,10 +5969,10 @@
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="1" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C271" s="1" t="s">
         <v>27</v>
@@ -5980,10 +5983,10 @@
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="1" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="C272" s="1" t="s">
         <v>27</v>
@@ -5994,10 +5997,10 @@
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="1" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="C273" s="1" t="s">
         <v>27</v>
@@ -6008,10 +6011,10 @@
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="1" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="C274" s="1" t="s">
         <v>30</v>
@@ -6022,10 +6025,10 @@
     </row>
     <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="1" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C275" s="1" t="s">
         <v>41</v>
@@ -6036,10 +6039,10 @@
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="1" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C276" s="1" t="s">
         <v>41</v>
@@ -6050,10 +6053,10 @@
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="1" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="C277" s="1" t="s">
         <v>41</v>
@@ -6064,10 +6067,10 @@
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="1" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="C278" s="1" t="s">
         <v>30</v>
@@ -6078,10 +6081,10 @@
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="1" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="C279" s="1" t="s">
         <v>41</v>
@@ -6092,13 +6095,13 @@
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="1" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="C280" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D280" s="1" t="s">
         <v>3</v>
@@ -6106,10 +6109,10 @@
     </row>
     <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="1" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="C281" s="1" t="s">
         <v>41</v>
@@ -6120,10 +6123,10 @@
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="1" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="C282" s="1" t="s">
         <v>30</v>
@@ -6134,10 +6137,10 @@
     </row>
     <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="C283" s="1" t="s">
         <v>41</v>
@@ -6151,10 +6154,10 @@
     </row>
     <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="1" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C284" s="1" t="s">
         <v>27</v>
@@ -6165,10 +6168,10 @@
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="1" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="C285" s="1" t="s">
         <v>30</v>
@@ -6179,10 +6182,10 @@
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="1" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="C286" s="1" t="s">
         <v>30</v>
@@ -6193,13 +6196,13 @@
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="1" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="C287" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D287" s="1" t="s">
         <v>3</v>
@@ -6207,13 +6210,13 @@
     </row>
     <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="1" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="C288" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D288" s="1" t="s">
         <v>3</v>
@@ -6221,10 +6224,10 @@
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="1" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="C289" s="1" t="s">
         <v>30</v>
@@ -6235,10 +6238,10 @@
     </row>
     <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="1" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="C290" s="1" t="s">
         <v>30</v>
@@ -6249,10 +6252,10 @@
     </row>
     <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="1" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="C291" s="1" t="s">
         <v>41</v>
@@ -6263,10 +6266,10 @@
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="1" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="C292" s="1" t="s">
         <v>30</v>
@@ -6277,10 +6280,10 @@
     </row>
     <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="1" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="C293" s="1" t="s">
         <v>41</v>
@@ -6291,10 +6294,10 @@
     </row>
     <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="1" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="C294" s="1" t="s">
         <v>30</v>
@@ -6305,13 +6308,13 @@
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="1" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="C295" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D295" s="1" t="s">
         <v>3</v>
@@ -6319,13 +6322,13 @@
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="1" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="C296" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D296" s="1" t="s">
         <v>3</v>
@@ -6333,10 +6336,10 @@
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="1" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="C297" s="1" t="s">
         <v>41</v>
@@ -6347,10 +6350,10 @@
     </row>
     <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="1" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="C298" s="1" t="s">
         <v>27</v>
@@ -6361,10 +6364,10 @@
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="1" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="C299" s="1" t="s">
         <v>30</v>
@@ -6375,10 +6378,10 @@
     </row>
     <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="1" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="C300" s="1" t="s">
         <v>30</v>
@@ -6389,10 +6392,10 @@
     </row>
     <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="1" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="C301" s="1" t="s">
         <v>27</v>
@@ -6403,10 +6406,10 @@
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="C302" s="1" t="s">
         <v>30</v>
@@ -6420,10 +6423,10 @@
     </row>
     <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="1" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="C303" s="1" t="s">
         <v>30</v>
@@ -6434,10 +6437,10 @@
     </row>
     <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="1" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="C304" s="1" t="s">
         <v>30</v>
@@ -6448,10 +6451,10 @@
     </row>
     <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="1" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="C305" s="1" t="s">
         <v>30</v>
@@ -6462,10 +6465,10 @@
     </row>
     <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="1" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="C306" s="1" t="s">
         <v>30</v>
@@ -6476,10 +6479,10 @@
     </row>
     <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="1" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="C307" s="1" t="s">
         <v>30</v>
@@ -6490,10 +6493,10 @@
     </row>
     <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="1" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C308" s="1" t="s">
         <v>41</v>
@@ -6504,10 +6507,10 @@
     </row>
     <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="1" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="C309" s="1" t="s">
         <v>27</v>
@@ -6518,10 +6521,10 @@
     </row>
     <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="1" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="C310" s="1" t="s">
         <v>41</v>
@@ -6532,10 +6535,10 @@
     </row>
     <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="1" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="C311" s="1" t="s">
         <v>27</v>
@@ -6546,10 +6549,10 @@
     </row>
     <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="1" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="C312" s="1" t="s">
         <v>30</v>
@@ -6563,13 +6566,13 @@
     </row>
     <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="1" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C313" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D313" s="1" t="s">
         <v>3</v>
@@ -6577,13 +6580,13 @@
     </row>
     <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="1" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="C314" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D314" s="1" t="s">
         <v>3</v>
@@ -6591,13 +6594,13 @@
     </row>
     <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="1" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="B315" s="1" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="C315" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D315" s="1" t="s">
         <v>3</v>
@@ -6605,13 +6608,13 @@
     </row>
     <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="1" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="C316" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D316" s="1" t="s">
         <v>3</v>
@@ -6619,10 +6622,10 @@
     </row>
     <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="1" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="C317" s="1" t="s">
         <v>27</v>
@@ -6633,10 +6636,10 @@
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="1" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="C318" s="1" t="s">
         <v>41</v>
@@ -6647,13 +6650,13 @@
     </row>
     <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="1" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="C319" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D319" s="1" t="s">
         <v>3</v>
@@ -6661,13 +6664,13 @@
     </row>
     <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="1" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="B320" s="1" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="C320" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D320" s="1" t="s">
         <v>3</v>
@@ -6675,10 +6678,10 @@
     </row>
     <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="1" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="C321" s="1" t="s">
         <v>41</v>
@@ -6689,10 +6692,10 @@
     </row>
     <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="1" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="C322" s="1" t="s">
         <v>30</v>
@@ -6703,10 +6706,10 @@
     </row>
     <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="C323" s="1" t="s">
         <v>30</v>
@@ -6720,10 +6723,10 @@
     </row>
     <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="1" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="C324" s="1" t="s">
         <v>2</v>
@@ -6737,10 +6740,10 @@
     </row>
     <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="1" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="C325" s="1" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
se arregla lo de la tabla con otros defectos
</commit_message>
<xml_diff>
--- a/app/templates/template_rules_1.xlsx
+++ b/app/templates/template_rules_1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1359" uniqueCount="630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="610">
   <si>
     <t xml:space="preserve">Certificado conformidad MINVU.</t>
   </si>
@@ -238,12 +238,6 @@
     <t xml:space="preserve">1.14.1</t>
   </si>
   <si>
-    <t xml:space="preserve">Especificar.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.15.1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sala de máquinas o de poleas no reservado sólo a personal autorizado.</t>
   </si>
   <si>
@@ -487,12 +481,6 @@
     <t xml:space="preserve">2.16.1</t>
   </si>
   <si>
-    <t xml:space="preserve">(Especificar).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.17.1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Puertas de piso de dimensiones no reglamentarias</t>
   </si>
   <si>
@@ -736,12 +724,6 @@
     <t xml:space="preserve">3.14.1</t>
   </si>
   <si>
-    <t xml:space="preserve">Especificar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.15.1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Paredes, techo y estructura de piso de cabina no reglamentario</t>
   </si>
   <si>
@@ -1027,12 +1009,6 @@
     <t xml:space="preserve">4.14.7</t>
   </si>
   <si>
-    <t xml:space="preserve">(Especificar)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.15.1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cable(s) suspensión con un torón roto o alambres rotos en un paso.</t>
   </si>
   <si>
@@ -1315,9 +1291,6 @@
     <t xml:space="preserve">5.15.3</t>
   </si>
   <si>
-    <t xml:space="preserve">5.18.1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Características no reglamentarias de los rieles guía de cabina. </t>
   </si>
   <si>
@@ -1411,9 +1384,6 @@
     <t xml:space="preserve">6.6.2</t>
   </si>
   <si>
-    <t xml:space="preserve">6.7.1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Holguras cabina – recinto inferiores a las reglamentarias en ascensores sin puerta en cabina (especificar).</t>
   </si>
   <si>
@@ -1432,12 +1402,6 @@
     <t xml:space="preserve">7.3.1</t>
   </si>
   <si>
-    <t xml:space="preserve">7.4.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vi, DI</t>
-  </si>
-  <si>
     <t xml:space="preserve">Existencia de desgaste excesivo de superficies consumibles del sistema de freno (especificar)</t>
   </si>
   <si>
@@ -1588,9 +1552,6 @@
     <t xml:space="preserve">8.14.1</t>
   </si>
   <si>
-    <t xml:space="preserve">8.16.1</t>
-  </si>
-  <si>
     <t xml:space="preserve">La superficie de trabajo en techo de cabina es menor 0,5 x 0,6 m.</t>
   </si>
   <si>
@@ -1687,9 +1648,6 @@
     <t xml:space="preserve">9.2.11.1</t>
   </si>
   <si>
-    <t xml:space="preserve">9.2.12.1</t>
-  </si>
-  <si>
     <t xml:space="preserve">9.3.1.1</t>
   </si>
   <si>
@@ -1774,9 +1732,6 @@
     <t xml:space="preserve">9.3.7.4</t>
   </si>
   <si>
-    <t xml:space="preserve">9.3.8.1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Inexistencia de armario de la maquinaria.</t>
   </si>
   <si>
@@ -1831,12 +1786,6 @@
     <t xml:space="preserve">9.4.2.1</t>
   </si>
   <si>
-    <t xml:space="preserve">(Especificar) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.4.3.1</t>
-  </si>
-  <si>
     <t xml:space="preserve">No existe continuidad de tierra o conexiones no reglamentarias.</t>
   </si>
   <si>
@@ -1897,19 +1846,10 @@
     <t xml:space="preserve">10.7.1</t>
   </si>
   <si>
-    <t xml:space="preserve">10.9.1</t>
-  </si>
-  <si>
     <t xml:space="preserve">El ascensor no cumple la reglamentación (desviaciones particulares) con la que fue puesto en servicio, y no existe constancia documental que justifique dicho incumplimiento (especificar).</t>
   </si>
   <si>
     <t xml:space="preserve">11.1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (especificar).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11.2.1</t>
   </si>
 </sst>
 </file>
@@ -2020,10 +1960,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E325"/>
+  <dimension ref="A1:E312"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A235" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A78" activeCellId="0" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2562,13 +2502,10 @@
         <v>73</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2607,7 +2544,7 @@
         <v>79</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>3</v>
@@ -2691,7 +2628,7 @@
         <v>91</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>3</v>
@@ -2719,7 +2656,7 @@
         <v>95</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>3</v>
@@ -2733,7 +2670,7 @@
         <v>97</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>3</v>
@@ -2747,7 +2684,7 @@
         <v>99</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>3</v>
@@ -2761,7 +2698,7 @@
         <v>101</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>3</v>
@@ -2817,7 +2754,7 @@
         <v>109</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>3</v>
@@ -2845,7 +2782,7 @@
         <v>113</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>3</v>
@@ -2859,7 +2796,7 @@
         <v>115</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>3</v>
@@ -2873,7 +2810,7 @@
         <v>117</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>3</v>
@@ -2887,7 +2824,7 @@
         <v>119</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>3</v>
@@ -2929,7 +2866,7 @@
         <v>125</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>3</v>
@@ -2940,7 +2877,7 @@
         <v>126</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>41</v>
@@ -2951,10 +2888,10 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>41</v>
@@ -2996,7 +2933,7 @@
         <v>133</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>41</v>
@@ -3007,13 +2944,13 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="C68" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>3</v>
@@ -3041,7 +2978,7 @@
         <v>139</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>3</v>
@@ -3052,10 +2989,10 @@
         <v>140</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>3</v>
@@ -3063,16 +3000,19 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B72" s="1" t="s">
-        <v>141</v>
-      </c>
       <c r="C72" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3083,13 +3023,10 @@
         <v>144</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3133,6 +3070,9 @@
       <c r="D76" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E76" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
@@ -3147,9 +3087,6 @@
       <c r="D77" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E77" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
@@ -3173,13 +3110,10 @@
         <v>156</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3190,7 +3124,7 @@
         <v>158</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>3</v>
@@ -3204,7 +3138,7 @@
         <v>160</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>3</v>
@@ -3248,8 +3182,8 @@
       <c r="C84" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D84" s="1" t="s">
-        <v>3</v>
+      <c r="E84" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3274,10 +3208,10 @@
         <v>170</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3285,10 +3219,10 @@
         <v>171</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>3</v>
@@ -3296,21 +3230,21 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D88" s="1" t="s">
-        <v>3</v>
+      <c r="E88" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>174</v>
@@ -3324,27 +3258,27 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B90" s="1" t="s">
-        <v>174</v>
-      </c>
       <c r="C90" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>4</v>
+        <v>177</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>3</v>
@@ -3352,16 +3286,16 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>3</v>
+        <v>30</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3388,6 +3322,9 @@
       <c r="C94" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="D94" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="E94" s="1" t="s">
         <v>4</v>
       </c>
@@ -3400,10 +3337,10 @@
         <v>187</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>3</v>
+        <v>30</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3414,13 +3351,10 @@
         <v>189</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3431,10 +3365,10 @@
         <v>191</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>4</v>
+        <v>41</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3445,35 +3379,41 @@
         <v>193</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>3</v>
+        <v>27</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B99" s="1" t="s">
-        <v>195</v>
-      </c>
       <c r="C99" s="1" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B100" s="1" t="s">
-        <v>197</v>
-      </c>
       <c r="C100" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>4</v>
@@ -3481,19 +3421,16 @@
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>198</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3504,10 +3441,7 @@
         <v>200</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>4</v>
@@ -3535,7 +3469,10 @@
         <v>204</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>4</v>
@@ -3563,10 +3500,7 @@
         <v>208</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>4</v>
@@ -3582,8 +3516,8 @@
       <c r="C107" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D107" s="1" t="s">
-        <v>3</v>
+      <c r="E107" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3594,10 +3528,10 @@
         <v>212</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E108" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3608,10 +3542,10 @@
         <v>214</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3622,10 +3556,10 @@
         <v>216</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>3</v>
+        <v>41</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3636,10 +3570,10 @@
         <v>218</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>3</v>
+        <v>41</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3652,8 +3586,8 @@
       <c r="C112" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E112" s="1" t="s">
-        <v>4</v>
+      <c r="D112" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3664,10 +3598,10 @@
         <v>222</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E113" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3692,7 +3626,7 @@
         <v>226</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>3</v>
@@ -3706,7 +3640,7 @@
         <v>228</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>3</v>
@@ -3720,7 +3654,7 @@
         <v>230</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>41</v>
+        <v>231</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>3</v>
@@ -3728,27 +3662,27 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>3</v>
+        <v>41</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>235</v>
+        <v>27</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>3</v>
@@ -3762,10 +3696,10 @@
         <v>237</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E120" s="1" t="s">
-        <v>4</v>
+        <v>27</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3776,7 +3710,7 @@
         <v>239</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>3</v>
@@ -3807,7 +3741,7 @@
         <v>243</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>27</v>
+        <v>231</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>3</v>
@@ -3821,7 +3755,7 @@
         <v>245</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>27</v>
+        <v>231</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>3</v>
@@ -3838,7 +3772,7 @@
         <v>247</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>27</v>
+        <v>231</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>3</v>
@@ -3852,7 +3786,7 @@
         <v>249</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>235</v>
+        <v>30</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>3</v>
@@ -3866,13 +3800,10 @@
         <v>251</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>235</v>
+        <v>30</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E127" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3883,7 +3814,7 @@
         <v>253</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>235</v>
+        <v>30</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>3</v>
@@ -3922,55 +3853,58 @@
         <v>258</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D131" s="1" t="s">
-        <v>3</v>
+      <c r="E131" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B132" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B132" s="1" t="s">
-        <v>261</v>
-      </c>
       <c r="C132" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D132" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B133" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="B133" s="1" t="s">
-        <v>263</v>
-      </c>
       <c r="C133" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D133" s="1" t="s">
-        <v>3</v>
+      <c r="E133" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B134" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="B134" s="1" t="s">
-        <v>263</v>
-      </c>
       <c r="C134" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E134" s="1" t="s">
-        <v>4</v>
+      <c r="D134" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3981,7 +3915,7 @@
         <v>266</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="D135" s="1" t="s">
         <v>3</v>
@@ -3998,7 +3932,10 @@
         <v>268</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>4</v>
@@ -4012,10 +3949,13 @@
         <v>270</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D137" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4031,9 +3971,6 @@
       <c r="D138" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E138" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="s">
@@ -4043,7 +3980,7 @@
         <v>274</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>41</v>
+        <v>275</v>
       </c>
       <c r="D139" s="1" t="s">
         <v>3</v>
@@ -4054,30 +3991,27 @@
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D140" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E140" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D141" s="1" t="s">
         <v>3</v>
@@ -4085,19 +4019,16 @@
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>281</v>
+        <v>27</v>
       </c>
       <c r="D142" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E142" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4124,8 +4055,8 @@
       <c r="C144" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D144" s="1" t="s">
-        <v>3</v>
+      <c r="E144" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4136,10 +4067,10 @@
         <v>287</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D145" s="1" t="s">
-        <v>3</v>
+        <v>30</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4150,10 +4081,10 @@
         <v>289</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D146" s="1" t="s">
-        <v>3</v>
+        <v>41</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4161,24 +4092,27 @@
         <v>290</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E147" s="1" t="s">
-        <v>4</v>
+        <v>41</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B148" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="B148" s="1" t="s">
-        <v>293</v>
-      </c>
       <c r="C148" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="E148" s="1" t="s">
         <v>4</v>
@@ -4186,10 +4120,10 @@
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B149" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="B149" s="1" t="s">
-        <v>295</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>41</v>
@@ -4200,16 +4134,16 @@
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B150" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="B150" s="1" t="s">
-        <v>295</v>
-      </c>
       <c r="C150" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D150" s="1" t="s">
-        <v>3</v>
+      <c r="E150" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4225,9 +4159,6 @@
       <c r="D151" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E151" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="1" t="s">
@@ -4239,8 +4170,8 @@
       <c r="C152" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E152" s="1" t="s">
-        <v>4</v>
+      <c r="D152" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4253,8 +4184,8 @@
       <c r="C153" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E153" s="1" t="s">
-        <v>4</v>
+      <c r="D153" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4307,7 +4238,7 @@
         <v>310</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="D157" s="1" t="s">
         <v>3</v>
@@ -4321,7 +4252,7 @@
         <v>312</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D158" s="1" t="s">
         <v>3</v>
@@ -4332,10 +4263,10 @@
         <v>313</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D159" s="1" t="s">
         <v>3</v>
@@ -4343,13 +4274,13 @@
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B160" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="B160" s="1" t="s">
-        <v>316</v>
-      </c>
       <c r="C160" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>3</v>
@@ -4357,10 +4288,10 @@
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B161" s="1" t="s">
         <v>317</v>
-      </c>
-      <c r="B161" s="1" t="s">
-        <v>318</v>
       </c>
       <c r="C161" s="1" t="s">
         <v>30</v>
@@ -4371,10 +4302,10 @@
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B162" s="1" t="s">
         <v>319</v>
-      </c>
-      <c r="B162" s="1" t="s">
-        <v>318</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>30</v>
@@ -4391,7 +4322,7 @@
         <v>321</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D163" s="1" t="s">
         <v>3</v>
@@ -4413,10 +4344,10 @@
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B165" s="1" t="s">
         <v>324</v>
-      </c>
-      <c r="B165" s="1" t="s">
-        <v>325</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>30</v>
@@ -4427,10 +4358,10 @@
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B166" s="1" t="s">
         <v>326</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>327</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>30</v>
@@ -4441,30 +4372,33 @@
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B167" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="B167" s="1" t="s">
-        <v>329</v>
-      </c>
       <c r="C167" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D167" s="1" t="s">
-        <v>3</v>
+      <c r="E167" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="1" t="s">
-        <v>269</v>
+        <v>329</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>330</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D168" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4475,10 +4409,13 @@
         <v>332</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D169" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4489,7 +4426,7 @@
         <v>334</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E170" s="1" t="s">
         <v>4</v>
@@ -4503,10 +4440,7 @@
         <v>336</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D171" s="1" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="E171" s="1" t="s">
         <v>4</v>
@@ -4520,13 +4454,10 @@
         <v>338</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D172" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E172" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4537,10 +4468,7 @@
         <v>340</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D173" s="1" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="E173" s="1" t="s">
         <v>4</v>
@@ -4554,7 +4482,10 @@
         <v>342</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="E174" s="1" t="s">
         <v>4</v>
@@ -4568,10 +4499,10 @@
         <v>344</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E175" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4582,7 +4513,7 @@
         <v>346</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D176" s="1" t="s">
         <v>3</v>
@@ -4598,8 +4529,8 @@
       <c r="C177" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E177" s="1" t="s">
-        <v>4</v>
+      <c r="D177" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4610,13 +4541,10 @@
         <v>350</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D178" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E178" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4629,8 +4557,8 @@
       <c r="C179" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D179" s="1" t="s">
-        <v>3</v>
+      <c r="E179" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4641,7 +4569,7 @@
         <v>354</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D180" s="1" t="s">
         <v>3</v>
@@ -4660,6 +4588,9 @@
       <c r="D181" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E181" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="1" t="s">
@@ -4674,6 +4605,9 @@
       <c r="D182" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E182" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="1" t="s">
@@ -4685,6 +4619,9 @@
       <c r="C183" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="D183" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="E183" s="1" t="s">
         <v>4</v>
       </c>
@@ -4697,7 +4634,7 @@
         <v>362</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D184" s="1" t="s">
         <v>3</v>
@@ -4711,7 +4648,7 @@
         <v>364</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D185" s="1" t="s">
         <v>3</v>
@@ -4728,13 +4665,10 @@
         <v>366</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="D186" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E186" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4750,9 +4684,6 @@
       <c r="D187" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E187" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="1" t="s">
@@ -4762,7 +4693,7 @@
         <v>370</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D188" s="1" t="s">
         <v>3</v>
@@ -4778,9 +4709,6 @@
       <c r="C189" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D189" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="E189" s="1" t="s">
         <v>4</v>
       </c>
@@ -4795,8 +4723,8 @@
       <c r="C190" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D190" s="1" t="s">
-        <v>3</v>
+      <c r="E190" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4807,10 +4735,10 @@
         <v>376</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D191" s="1" t="s">
-        <v>3</v>
+        <v>41</v>
+      </c>
+      <c r="E191" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4821,10 +4749,10 @@
         <v>378</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D192" s="1" t="s">
-        <v>3</v>
+        <v>41</v>
+      </c>
+      <c r="E192" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4849,7 +4777,7 @@
         <v>382</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="E194" s="1" t="s">
         <v>4</v>
@@ -4865,6 +4793,9 @@
       <c r="C195" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="D195" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="E195" s="1" t="s">
         <v>4</v>
       </c>
@@ -4879,8 +4810,8 @@
       <c r="C196" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E196" s="1" t="s">
-        <v>4</v>
+      <c r="D196" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4891,10 +4822,10 @@
         <v>388</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E197" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
+      </c>
+      <c r="D197" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4905,7 +4836,7 @@
         <v>390</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E198" s="1" t="s">
         <v>4</v>
@@ -4919,13 +4850,10 @@
         <v>392</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D199" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E199" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4936,10 +4864,10 @@
         <v>394</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D200" s="1" t="s">
-        <v>3</v>
+        <v>30</v>
+      </c>
+      <c r="E200" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4950,7 +4878,7 @@
         <v>396</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D201" s="1" t="s">
         <v>3</v>
@@ -4964,7 +4892,7 @@
         <v>398</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E202" s="1" t="s">
         <v>4</v>
@@ -4978,10 +4906,13 @@
         <v>400</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D203" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="E203" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4994,6 +4925,9 @@
       <c r="C204" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="D204" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="E204" s="1" t="s">
         <v>4</v>
       </c>
@@ -5006,10 +4940,13 @@
         <v>404</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D205" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="E205" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5020,7 +4957,10 @@
         <v>406</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
+      </c>
+      <c r="D206" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="E206" s="1" t="s">
         <v>4</v>
@@ -5034,13 +4974,10 @@
         <v>408</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>27</v>
+        <v>275</v>
       </c>
       <c r="D207" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E207" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5051,10 +4988,7 @@
         <v>410</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D208" s="1" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="E208" s="1" t="s">
         <v>4</v>
@@ -5068,10 +5002,7 @@
         <v>412</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D209" s="1" t="s">
-        <v>3</v>
+        <v>275</v>
       </c>
       <c r="E209" s="1" t="s">
         <v>4</v>
@@ -5102,10 +5033,13 @@
         <v>416</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>281</v>
+        <v>41</v>
       </c>
       <c r="D211" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="E211" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5130,7 +5064,7 @@
         <v>420</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>281</v>
+        <v>41</v>
       </c>
       <c r="E213" s="1" t="s">
         <v>4</v>
@@ -5149,9 +5083,6 @@
       <c r="D214" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E214" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="1" t="s">
@@ -5161,13 +5092,10 @@
         <v>424</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D215" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E215" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5178,10 +5106,10 @@
         <v>426</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E216" s="1" t="s">
-        <v>4</v>
+        <v>27</v>
+      </c>
+      <c r="D216" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5192,10 +5120,10 @@
         <v>428</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E217" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
+      </c>
+      <c r="D217" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5206,35 +5134,35 @@
         <v>430</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D218" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="E218" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="1" t="s">
-        <v>155</v>
+        <v>431</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="D219" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E219" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="1" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C220" s="1" t="s">
         <v>30</v>
@@ -5245,13 +5173,13 @@
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="1" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D221" s="1" t="s">
         <v>3</v>
@@ -5259,13 +5187,13 @@
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="1" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D222" s="1" t="s">
         <v>3</v>
@@ -5273,30 +5201,27 @@
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D223" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E223" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="B224" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="B224" s="1" t="s">
-        <v>441</v>
-      </c>
       <c r="C224" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="D224" s="1" t="s">
         <v>3</v>
@@ -5310,7 +5235,7 @@
         <v>443</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D225" s="1" t="s">
         <v>3</v>
@@ -5324,10 +5249,10 @@
         <v>445</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D226" s="1" t="s">
-        <v>3</v>
+        <v>41</v>
+      </c>
+      <c r="E226" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5338,7 +5263,7 @@
         <v>447</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D227" s="1" t="s">
         <v>3</v>
@@ -5363,52 +5288,52 @@
         <v>450</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="C229" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D229" s="1" t="s">
-        <v>3</v>
+      <c r="E229" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="1" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C230" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D230" s="1" t="s">
-        <v>3</v>
+      <c r="E230" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="1" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E231" s="1" t="s">
-        <v>4</v>
+        <v>27</v>
+      </c>
+      <c r="D231" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D232" s="1" t="s">
         <v>3</v>
@@ -5416,13 +5341,13 @@
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="D233" s="1" t="s">
         <v>3</v>
@@ -5430,13 +5355,16 @@
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="1" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
+      </c>
+      <c r="D234" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="E234" s="1" t="s">
         <v>4</v>
@@ -5444,10 +5372,10 @@
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="1" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>41</v>
@@ -5458,30 +5386,27 @@
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="1" t="s">
-        <v>155</v>
+        <v>464</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D236" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E236" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="1" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D237" s="1" t="s">
         <v>3</v>
@@ -5489,27 +5414,27 @@
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="1" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D238" s="1" t="s">
-        <v>3</v>
+        <v>30</v>
+      </c>
+      <c r="E238" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="1" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D239" s="1" t="s">
         <v>3</v>
@@ -5517,16 +5442,13 @@
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="1" t="s">
-        <v>155</v>
+        <v>472</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="D240" s="1" t="s">
-        <v>3</v>
+        <v>275</v>
       </c>
       <c r="E240" s="1" t="s">
         <v>4</v>
@@ -5534,13 +5456,13 @@
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="1" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>30</v>
+        <v>275</v>
       </c>
       <c r="D241" s="1" t="s">
         <v>3</v>
@@ -5551,27 +5473,27 @@
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="1" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E242" s="1" t="s">
-        <v>4</v>
+        <v>177</v>
+      </c>
+      <c r="D242" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="1" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D243" s="1" t="s">
         <v>3</v>
@@ -5579,13 +5501,13 @@
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="1" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D244" s="1" t="s">
         <v>3</v>
@@ -5593,27 +5515,27 @@
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="1" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E245" s="1" t="s">
-        <v>4</v>
+        <v>41</v>
+      </c>
+      <c r="D245" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="1" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D246" s="1" t="s">
         <v>3</v>
@@ -5621,44 +5543,41 @@
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="1" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="E247" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
+      </c>
+      <c r="D247" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="1" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>281</v>
+        <v>30</v>
       </c>
       <c r="D248" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E248" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="1" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>181</v>
+        <v>41</v>
       </c>
       <c r="D249" s="1" t="s">
         <v>3</v>
@@ -5666,10 +5585,10 @@
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="1" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="C250" s="1" t="s">
         <v>41</v>
@@ -5680,24 +5599,24 @@
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="1" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="C251" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D251" s="1" t="s">
-        <v>3</v>
+      <c r="E251" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="1" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="C252" s="1" t="s">
         <v>41</v>
@@ -5708,13 +5627,13 @@
     </row>
     <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="1" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="C253" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="D253" s="1" t="s">
         <v>3</v>
@@ -5722,10 +5641,10 @@
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="1" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="C254" s="1" t="s">
         <v>30</v>
@@ -5736,10 +5655,10 @@
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="1" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="C255" s="1" t="s">
         <v>30</v>
@@ -5750,55 +5669,61 @@
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="1" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="C256" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D256" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="E256" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="1" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>41</v>
+        <v>275</v>
       </c>
       <c r="D257" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="E257" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="1" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E258" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
+      </c>
+      <c r="D258" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="1" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="C259" s="1" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="D259" s="1" t="s">
         <v>3</v>
@@ -5806,13 +5731,13 @@
     </row>
     <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="1" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="C260" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D260" s="1" t="s">
         <v>3</v>
@@ -5820,10 +5745,10 @@
     </row>
     <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="1" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="C261" s="1" t="s">
         <v>30</v>
@@ -5834,61 +5759,55 @@
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="1" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="C262" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D262" s="1" t="s">
-        <v>3</v>
+      <c r="E262" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="1" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="D263" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E263" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="1" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>281</v>
+        <v>27</v>
       </c>
       <c r="D264" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E264" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="1" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="C265" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D265" s="1" t="s">
         <v>3</v>
@@ -5896,30 +5815,27 @@
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="1" t="s">
-        <v>155</v>
+        <v>524</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="C266" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D266" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E266" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="1" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="C267" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="D267" s="1" t="s">
         <v>3</v>
@@ -5927,13 +5843,13 @@
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="1" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="C268" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D268" s="1" t="s">
         <v>3</v>
@@ -5941,13 +5857,13 @@
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="1" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="C269" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D269" s="1" t="s">
         <v>3</v>
@@ -5955,27 +5871,27 @@
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="1" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="C270" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E270" s="1" t="s">
-        <v>4</v>
+      <c r="D270" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="1" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="C271" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="D271" s="1" t="s">
         <v>3</v>
@@ -5983,13 +5899,13 @@
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="1" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="C272" s="1" t="s">
-        <v>27</v>
+        <v>177</v>
       </c>
       <c r="D272" s="1" t="s">
         <v>3</v>
@@ -5997,13 +5913,13 @@
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="1" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="C273" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="D273" s="1" t="s">
         <v>3</v>
@@ -6011,10 +5927,10 @@
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="1" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="C274" s="1" t="s">
         <v>30</v>
@@ -6025,13 +5941,13 @@
     </row>
     <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="1" t="s">
-        <v>539</v>
+        <v>510</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="C275" s="1" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="D275" s="1" t="s">
         <v>3</v>
@@ -6039,13 +5955,13 @@
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="1" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="C276" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D276" s="1" t="s">
         <v>3</v>
@@ -6053,27 +5969,27 @@
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="1" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="C277" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D277" s="1" t="s">
-        <v>3</v>
+        <v>30</v>
+      </c>
+      <c r="E277" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="1" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>30</v>
+        <v>231</v>
       </c>
       <c r="D278" s="1" t="s">
         <v>3</v>
@@ -6081,13 +5997,13 @@
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="1" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="C279" s="1" t="s">
-        <v>41</v>
+        <v>231</v>
       </c>
       <c r="D279" s="1" t="s">
         <v>3</v>
@@ -6095,13 +6011,13 @@
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="1" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="C280" s="1" t="s">
-        <v>181</v>
+        <v>30</v>
       </c>
       <c r="D280" s="1" t="s">
         <v>3</v>
@@ -6109,13 +6025,13 @@
     </row>
     <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="1" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="C281" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D281" s="1" t="s">
         <v>3</v>
@@ -6123,13 +6039,13 @@
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="1" t="s">
-        <v>553</v>
+        <v>526</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="C282" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D282" s="1" t="s">
         <v>3</v>
@@ -6137,30 +6053,27 @@
     </row>
     <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="1" t="s">
-        <v>155</v>
+        <v>528</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C283" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D283" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E283" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="1" t="s">
-        <v>523</v>
+        <v>557</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="C284" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="D284" s="1" t="s">
         <v>3</v>
@@ -6168,10 +6081,10 @@
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="1" t="s">
-        <v>557</v>
+        <v>532</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C285" s="1" t="s">
         <v>30</v>
@@ -6182,27 +6095,27 @@
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="1" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="C286" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E286" s="1" t="s">
-        <v>4</v>
+        <v>275</v>
+      </c>
+      <c r="D286" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="1" t="s">
-        <v>561</v>
+        <v>536</v>
       </c>
       <c r="B287" s="1" t="s">
         <v>562</v>
       </c>
       <c r="C287" s="1" t="s">
-        <v>235</v>
+        <v>177</v>
       </c>
       <c r="D287" s="1" t="s">
         <v>3</v>
@@ -6210,13 +6123,13 @@
     </row>
     <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="B288" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="B288" s="1" t="s">
-        <v>564</v>
-      </c>
       <c r="C288" s="1" t="s">
-        <v>235</v>
+        <v>41</v>
       </c>
       <c r="D288" s="1" t="s">
         <v>3</v>
@@ -6224,13 +6137,13 @@
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="B289" s="1" t="s">
         <v>565</v>
       </c>
-      <c r="B289" s="1" t="s">
-        <v>566</v>
-      </c>
       <c r="C289" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D289" s="1" t="s">
         <v>3</v>
@@ -6238,10 +6151,10 @@
     </row>
     <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="1" t="s">
-        <v>567</v>
+        <v>514</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C290" s="1" t="s">
         <v>30</v>
@@ -6252,27 +6165,27 @@
     </row>
     <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="1" t="s">
-        <v>539</v>
+        <v>567</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C291" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D291" s="1" t="s">
-        <v>3</v>
+        <v>30</v>
+      </c>
+      <c r="E291" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="1" t="s">
-        <v>541</v>
+        <v>518</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C292" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D292" s="1" t="s">
         <v>3</v>
@@ -6280,13 +6193,13 @@
     </row>
     <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="B293" s="1" t="s">
         <v>571</v>
       </c>
-      <c r="B293" s="1" t="s">
-        <v>572</v>
-      </c>
       <c r="C293" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D293" s="1" t="s">
         <v>3</v>
@@ -6294,7 +6207,7 @@
     </row>
     <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="1" t="s">
-        <v>545</v>
+        <v>572</v>
       </c>
       <c r="B294" s="1" t="s">
         <v>573</v>
@@ -6314,7 +6227,7 @@
         <v>575</v>
       </c>
       <c r="C295" s="1" t="s">
-        <v>281</v>
+        <v>30</v>
       </c>
       <c r="D295" s="1" t="s">
         <v>3</v>
@@ -6322,13 +6235,13 @@
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="1" t="s">
-        <v>549</v>
+        <v>576</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="C296" s="1" t="s">
-        <v>181</v>
+        <v>30</v>
       </c>
       <c r="D296" s="1" t="s">
         <v>3</v>
@@ -6336,13 +6249,13 @@
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="1" t="s">
-        <v>551</v>
+        <v>578</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="C297" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D297" s="1" t="s">
         <v>3</v>
@@ -6350,13 +6263,13 @@
     </row>
     <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="1" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="C298" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="D298" s="1" t="s">
         <v>3</v>
@@ -6364,13 +6277,13 @@
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="1" t="s">
-        <v>527</v>
+        <v>582</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>580</v>
+        <v>583</v>
       </c>
       <c r="C299" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D299" s="1" t="s">
         <v>3</v>
@@ -6378,24 +6291,24 @@
     </row>
     <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="1" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>582</v>
+        <v>585</v>
       </c>
       <c r="C300" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E300" s="1" t="s">
-        <v>4</v>
+        <v>41</v>
+      </c>
+      <c r="D300" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="1" t="s">
-        <v>531</v>
+        <v>586</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>583</v>
+        <v>587</v>
       </c>
       <c r="C301" s="1" t="s">
         <v>27</v>
@@ -6406,30 +6319,27 @@
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="1" t="s">
-        <v>335</v>
+        <v>588</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>584</v>
+        <v>589</v>
       </c>
       <c r="C302" s="1" t="s">
-        <v>30</v>
+        <v>231</v>
       </c>
       <c r="D302" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E302" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="1" t="s">
-        <v>585</v>
+        <v>590</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>586</v>
+        <v>591</v>
       </c>
       <c r="C303" s="1" t="s">
-        <v>30</v>
+        <v>231</v>
       </c>
       <c r="D303" s="1" t="s">
         <v>3</v>
@@ -6437,13 +6347,13 @@
     </row>
     <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="1" t="s">
-        <v>587</v>
+        <v>592</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>588</v>
+        <v>593</v>
       </c>
       <c r="C304" s="1" t="s">
-        <v>30</v>
+        <v>231</v>
       </c>
       <c r="D304" s="1" t="s">
         <v>3</v>
@@ -6451,13 +6361,13 @@
     </row>
     <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="1" t="s">
-        <v>589</v>
+        <v>594</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
       <c r="C305" s="1" t="s">
-        <v>30</v>
+        <v>231</v>
       </c>
       <c r="D305" s="1" t="s">
         <v>3</v>
@@ -6465,13 +6375,13 @@
     </row>
     <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="1" t="s">
-        <v>591</v>
+        <v>596</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>592</v>
+        <v>597</v>
       </c>
       <c r="C306" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D306" s="1" t="s">
         <v>3</v>
@@ -6479,13 +6389,13 @@
     </row>
     <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="1" t="s">
-        <v>593</v>
+        <v>598</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>594</v>
+        <v>599</v>
       </c>
       <c r="C307" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D307" s="1" t="s">
         <v>3</v>
@@ -6493,13 +6403,13 @@
     </row>
     <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="1" t="s">
-        <v>595</v>
+        <v>600</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>596</v>
+        <v>601</v>
       </c>
       <c r="C308" s="1" t="s">
-        <v>41</v>
+        <v>275</v>
       </c>
       <c r="D308" s="1" t="s">
         <v>3</v>
@@ -6507,13 +6417,13 @@
     </row>
     <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="1" t="s">
-        <v>597</v>
+        <v>602</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>598</v>
+        <v>603</v>
       </c>
       <c r="C309" s="1" t="s">
-        <v>27</v>
+        <v>275</v>
       </c>
       <c r="D309" s="1" t="s">
         <v>3</v>
@@ -6521,10 +6431,10 @@
     </row>
     <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="1" t="s">
-        <v>599</v>
+        <v>604</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>600</v>
+        <v>605</v>
       </c>
       <c r="C310" s="1" t="s">
         <v>41</v>
@@ -6535,13 +6445,13 @@
     </row>
     <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="1" t="s">
-        <v>601</v>
+        <v>606</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>602</v>
+        <v>607</v>
       </c>
       <c r="C311" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D311" s="1" t="s">
         <v>3</v>
@@ -6549,209 +6459,18 @@
     </row>
     <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="1" t="s">
-        <v>603</v>
+        <v>608</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>604</v>
+        <v>609</v>
       </c>
       <c r="C312" s="1" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="D312" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E312" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A313" s="1" t="s">
-        <v>605</v>
-      </c>
-      <c r="B313" s="1" t="s">
-        <v>606</v>
-      </c>
-      <c r="C313" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="D313" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A314" s="1" t="s">
-        <v>607</v>
-      </c>
-      <c r="B314" s="1" t="s">
-        <v>608</v>
-      </c>
-      <c r="C314" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="D314" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A315" s="1" t="s">
-        <v>609</v>
-      </c>
-      <c r="B315" s="1" t="s">
-        <v>610</v>
-      </c>
-      <c r="C315" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="D315" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A316" s="1" t="s">
-        <v>611</v>
-      </c>
-      <c r="B316" s="1" t="s">
-        <v>612</v>
-      </c>
-      <c r="C316" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="D316" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A317" s="1" t="s">
-        <v>613</v>
-      </c>
-      <c r="B317" s="1" t="s">
-        <v>614</v>
-      </c>
-      <c r="C317" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D317" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A318" s="1" t="s">
-        <v>615</v>
-      </c>
-      <c r="B318" s="1" t="s">
-        <v>616</v>
-      </c>
-      <c r="C318" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D318" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A319" s="1" t="s">
-        <v>617</v>
-      </c>
-      <c r="B319" s="1" t="s">
-        <v>618</v>
-      </c>
-      <c r="C319" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="D319" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A320" s="1" t="s">
-        <v>619</v>
-      </c>
-      <c r="B320" s="1" t="s">
-        <v>620</v>
-      </c>
-      <c r="C320" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="D320" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A321" s="1" t="s">
-        <v>621</v>
-      </c>
-      <c r="B321" s="1" t="s">
-        <v>622</v>
-      </c>
-      <c r="C321" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D321" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A322" s="1" t="s">
-        <v>623</v>
-      </c>
-      <c r="B322" s="1" t="s">
-        <v>624</v>
-      </c>
-      <c r="C322" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D322" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A323" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B323" s="1" t="s">
-        <v>625</v>
-      </c>
-      <c r="C323" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D323" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E323" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A324" s="1" t="s">
-        <v>626</v>
-      </c>
-      <c r="B324" s="1" t="s">
-        <v>627</v>
-      </c>
-      <c r="C324" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D324" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E324" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A325" s="1" t="s">
-        <v>628</v>
-      </c>
-      <c r="B325" s="1" t="s">
-        <v>629</v>
-      </c>
-      <c r="C325" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D325" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E325" s="1" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se agrega funcion para actualizar el texto de un defecto para revision_nulls y revision_colors cuando se modifica el texto de un rule
</commit_message>
<xml_diff>
--- a/app/templates/template_rules_1.xlsx
+++ b/app/templates/template_rules_1.xlsx
@@ -1039,7 +1039,7 @@
     <t xml:space="preserve">5.2.1</t>
   </si>
   <si>
-    <t xml:space="preserve">Cacle de suspensión flojo con riesgo de desmonte de la garganta de la polea.</t>
+    <t xml:space="preserve">Cable de suspensión flojo con riesgo de desmonte de la garganta de la polea.</t>
   </si>
   <si>
     <t xml:space="preserve">5.2.2</t>
@@ -1962,8 +1962,8 @@
   </sheetPr>
   <dimension ref="A1:E312"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A235" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A78" activeCellId="0" sqref="A78"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A149" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A173" activeCellId="0" sqref="A173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>